<commit_message>
Added New migration file and changes in code
</commit_message>
<xml_diff>
--- a/cmarryRegistration.xlsx
+++ b/cmarryRegistration.xlsx
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>